<commit_message>
Content update after getting website working again
</commit_message>
<xml_diff>
--- a/content/species/data/nba_example_RLI_data_trim_freshwater.xlsx
+++ b/content/species/data/nba_example_RLI_data_trim_freshwater.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\nba-species\species\quarto\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\species\quarto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0E69E6-51CA-4B20-BAD6-993FE4A80947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4FD7D7-5E44-4FD3-B0B0-A36FD02FD6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" activeTab="1" xr2:uid="{027AC6A8-209D-4E42-8E53-EE844CC37963}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{027AC6A8-209D-4E42-8E53-EE844CC37963}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -69,13 +69,7 @@
     <t>Birds</t>
   </si>
   <si>
-    <t>Dragonflies</t>
-  </si>
-  <si>
     <t>Freshwater Crabs</t>
-  </si>
-  <si>
-    <t>Freshwater Fish</t>
   </si>
   <si>
     <t>Mammals</t>
@@ -91,6 +85,12 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>Dragonflies &amp; Damselflies</t>
+  </si>
+  <si>
+    <t>Freshwater Fishes</t>
   </si>
 </sst>
 </file>
@@ -941,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED362CF-FE85-44F6-BE1C-A838815FA964}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1113,7 +1113,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>2006</v>
@@ -1133,7 +1133,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>2018</v>
@@ -1153,7 +1153,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>2007</v>
@@ -1173,7 +1173,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>2025</v>
@@ -1193,7 +1193,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>2007</v>
@@ -1213,7 +1213,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>2017</v>
@@ -1233,7 +1233,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15">
         <v>2004</v>
@@ -1253,7 +1253,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B16">
         <v>2016</v>
@@ -1273,7 +1273,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>2025</v>
@@ -1293,7 +1293,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B18">
         <v>1990</v>
@@ -1313,7 +1313,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B19">
         <v>2018</v>
@@ -1333,7 +1333,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B20">
         <v>2025</v>
@@ -1353,7 +1353,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B21">
         <v>1990</v>
@@ -1373,7 +1373,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B22">
         <v>2018</v>
@@ -1393,7 +1393,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B23">
         <v>2022</v>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B24">
         <v>1990</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B25">
         <v>1991</v>
@@ -1453,7 +1453,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B26">
         <v>1992</v>
@@ -1473,7 +1473,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B27">
         <v>1993</v>
@@ -1493,7 +1493,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B28">
         <v>1994</v>
@@ -1513,7 +1513,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B29">
         <v>1995</v>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B30">
         <v>1996</v>
@@ -1553,7 +1553,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B31">
         <v>1997</v>
@@ -1573,7 +1573,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B32">
         <v>1998</v>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B33">
         <v>1999</v>
@@ -1613,7 +1613,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B34">
         <v>2000</v>
@@ -1633,7 +1633,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B35">
         <v>2001</v>
@@ -1653,7 +1653,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B36">
         <v>2002</v>
@@ -1673,7 +1673,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B37">
         <v>2003</v>
@@ -1693,7 +1693,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B38">
         <v>2004</v>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B39">
         <v>2005</v>
@@ -1733,7 +1733,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B40">
         <v>2006</v>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B41">
         <v>2007</v>
@@ -1773,7 +1773,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B42">
         <v>2008</v>
@@ -1793,7 +1793,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B43">
         <v>2009</v>
@@ -1813,7 +1813,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B44">
         <v>2010</v>
@@ -1833,7 +1833,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B45">
         <v>2011</v>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B46">
         <v>2012</v>
@@ -1873,7 +1873,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B47">
         <v>2013</v>
@@ -1893,7 +1893,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B48">
         <v>2014</v>
@@ -1913,7 +1913,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B49">
         <v>2015</v>
@@ -1933,7 +1933,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B50">
         <v>2016</v>
@@ -1953,7 +1953,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B51">
         <v>2017</v>
@@ -1973,7 +1973,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B52">
         <v>2018</v>
@@ -1993,7 +1993,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B53">
         <v>2019</v>
@@ -2013,7 +2013,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B54">
         <v>2020</v>
@@ -2033,7 +2033,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B55">
         <v>2021</v>
@@ -2053,7 +2053,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B56">
         <v>2022</v>
@@ -2073,7 +2073,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B57">
         <v>2023</v>
@@ -2093,7 +2093,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B58">
         <v>2024</v>
@@ -2113,7 +2113,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B59">
         <v>2025</v>
@@ -2141,13 +2141,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB69D90-1B21-4A37-827F-D250DE52680C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>